<commit_message>
cleaned up, added new functions
</commit_message>
<xml_diff>
--- a/Script Documentation.xlsx
+++ b/Script Documentation.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2502" uniqueCount="857">
   <si>
     <t>EXPRESSION_NAME</t>
   </si>
@@ -9393,48 +9393,6 @@
   </si>
   <si>
     <t>if (matches(currentUserID,"ADMIN", "LGAWAD")) { showDebug = false; } else { showDebug = false; /* enable debugging on on scripts for ADMIN userID */; } LICENSESTATE = "NY";</t>
-  </si>
-  <si>
-    <t>EMSE:LicProfLookup</t>
-  </si>
-  <si>
-    <t>logDebug("Using LICENSESTATE = " + LICENSESTATE + " from EMSE:GlobalFlags"); //Issue State; LICENSETYPE = ""; //License Type to be populated; licCapId = null; isNewLic = false; licIDString = null; licObj = null; licCap = null; branch("EMSE:LicProfLookup:getLicenses"); //Get License CAP; if (licCapId !=null) { branch("EMSE:LicProfLookup:getLicenseType"); } licObj = licenseProfObject(licIDString,LICENSETYPE); //Get LicArray; if (!licObj.valid &amp;&amp; lookup("LICENSED PROFESSIONAL TYPE",LICENSETYPE) != null) { branch("EMSE:LicProfLookup:CreateLP"); licObj = licenseProfObject(licIDString,LICENSETYPE ); } if (licObj.valid) { branch("EMSE:LicProfLookup:UpdateLP"); } else { logDebug("LP Not found to update"); }</t>
-  </si>
-  <si>
-    <t>EMSE:LicProfLookup:CreateLP</t>
-  </si>
-  <si>
-    <t>var vNewLic = aa.licenseScript.createLicenseScriptModel(); vNewLic.setAgencyCode(aa.getServiceProviderCode()); vNewLic.setAuditDate(sysDate); vNewLic.setAuditID(currentUserID); vNewLic.setAuditStatus("A"); vNewLic.setLicenseType(LICENSETYPE); vNewLic.setLicState(LICENSESTATE); vNewLic.setStateLicense(licIDString); aa.licenseScript.createRefLicenseProf(vNewLic); var tmpLicObj = licenseProfObject(licIDString,LICENSETYPE); if (tmpLicObj.valid) { isNewLic = true; }</t>
-  </si>
-  <si>
-    <t>EMSE:LicProfLookup:UpdateLP</t>
-  </si>
-  <si>
-    <t>branch("EMSE:LicProfLookup:UpdateLP:BaseFields"); branch("EMSE:LicProfLookup:UpdateLP:ApplicationStatus"); if (licObj.updateRecord()) { logDebug("LP Updated Successfully"); } else { logDebug("LP Update Failed"); }</t>
-  </si>
-  <si>
-    <t>EMSE:LicProfLookup:UpdateLP:ApplicationStatus</t>
-  </si>
-  <si>
-    <t>licObj.refLicModel.setBusinessName2(licCapStatus); logDebug("Lic Cap Status: " + licCapStatus);</t>
-  </si>
-  <si>
-    <t>EMSE:LicProfLookup:UpdateLP:BaseFields</t>
-  </si>
-  <si>
-    <t>licObj.refLicModel.setState(LICENSESTATE); licObj.refLicModel.setLicenseBoard(LICENSETYPE); licObj.refLicModel.setLicenseIssueDate(licCap.getFileDate()); var expObj = null; var expDt = null; var expObjRes = aa.expiration.getLicensesByCapID(licCapId); if(expObjRes.getSuccess()) var expObj = expObjRes.getOutput(); if (expObj != null) { expDt = aa.date.parseDate(expObj.getExpDateString()); } if (expDt != null) { licObj.refLicModel.setLicenseExpirationDate(expDt); //Expiration Date; } if (licCapTypeArr[1] == "Business") { licObj.refLicModel.setLicenseBoard(getAppSpecific("Business Type",licCapId)); } else { licObj.refLicModel.setLicenseBoard(LICENSETYPE); } if (licObj.updateFromRecordContactByType(licCapId,"",true,false);) { logDebug("LP Updated from Primary Contact"); } else { logDebug("LP Failed to Update from Primary Contact trying License Holder"); if(licObj.updateFromRecordContactByType(licCapId,"License Holder",true,false)) logDebug("Updated from License Holder"); else logDebug("Couldn't Update Contact Info"); } if (licObj.updateFromAddress(licCapId)) { logDebug("LP Address Updated from License Address"); } else { logDebug("LP Address Failed to update from License Address"); } if (getAppSpecific("Doing Business As (DBA) Name",licCapId)) { licObj.refLicModel.setBusinessName(getAppSpecific("Doing Business As (DBA) Name",licCapId) ); }</t>
-  </si>
-  <si>
-    <t>EMSE:LicProfLookup:getLicenseType</t>
-  </si>
-  <si>
-    <t>if (licCapId !=null) { licIDString = licCapId.getCustomID(); } if (licCapId !=null) { licCap = aa.cap.getCap(licCapId).getOutput(); licCapType = licCap.getCapType().toString(); licCapTypeArr = licCapType.split("/"); licCapStatus = licCap.getCapStatus(); } if (licCapId !=null) { LICENSETYPE = licCapTypeArr[2]; }</t>
-  </si>
-  <si>
-    <t>EMSE:LicProfLookup:getLicenses</t>
-  </si>
-  <si>
-    <t>var searchCap = capId; var tmpId = capId; var prjArr = null; if (appMatch("*/*/*/License")) { var childArr = getChildren("*/*/*/Application"); if(childArr != null) searchCap = childArr[0]; } capId = tmpId; var vRelationType = "R"; if(appMatch("*/*/*/Renewal")) vRelationType="Renewal"; var prjArrRes = aa.cap.getProjectByChildCapID(searchCap,vRelationType,null); if(prjArrRes.getSuccess()) prjArr = prjArrRes.getOutput(); if (prjArr != null) { for(prj in prjArr) if(appMatch("*/*/*/License",prjArr[prj].getProjectID())) licCapId = prjArr[prj].getProjectID(); } if (licCapId == null &amp;&amp; appMatch("*/*/*/License")) { licCapId = capId; //In the event license has no application; } if (licCapId != null) { licCapId = aa.cap.getCapID(licCapId.getID1(),licCapId.getID2(),licCapId.getID3()).getOutput(); logDebug("Got Lic Cap " + licCapId.getCustomID()); }</t>
   </si>
   <si>
     <t>EMSE_VariableBranching</t>
@@ -10609,8 +10567,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:B48" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="A1:B48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:B41" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="A1:B41"/>
   <sortState ref="A2:B55">
     <sortCondition ref="A1:A55"/>
   </sortState>
@@ -10933,7 +10891,7 @@
   <dimension ref="A1:K180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
@@ -16340,7 +16298,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17050,7 +17008,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17065,10 +17023,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>869</v>
+        <v>855</v>
       </c>
       <c r="B1" t="s">
-        <v>870</v>
+        <v>856</v>
       </c>
       <c r="C1" t="s">
         <v>564</v>
@@ -17085,7 +17043,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>868</v>
+        <v>854</v>
       </c>
       <c r="B2" t="s">
         <v>552</v>
@@ -17099,7 +17057,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>868</v>
+        <v>854</v>
       </c>
       <c r="B3" t="s">
         <v>552</v>
@@ -17113,7 +17071,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>868</v>
+        <v>854</v>
       </c>
       <c r="B4" t="s">
         <v>552</v>
@@ -17124,7 +17082,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>861</v>
+        <v>847</v>
       </c>
       <c r="B5" t="s">
         <v>514</v>
@@ -17132,9 +17090,6 @@
       <c r="C5" t="s">
         <v>515</v>
       </c>
-      <c r="D5" t="s">
-        <v>516</v>
-      </c>
       <c r="E5" t="s">
         <v>517</v>
       </c>
@@ -17144,7 +17099,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>861</v>
+        <v>847</v>
       </c>
       <c r="B6" t="s">
         <v>514</v>
@@ -17158,7 +17113,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>861</v>
+        <v>847</v>
       </c>
       <c r="B7" t="s">
         <v>514</v>
@@ -17175,7 +17130,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>861</v>
+        <v>847</v>
       </c>
       <c r="B8" t="s">
         <v>514</v>
@@ -17189,7 +17144,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>864</v>
+        <v>850</v>
       </c>
       <c r="B9" t="s">
         <v>534</v>
@@ -17203,7 +17158,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>864</v>
+        <v>850</v>
       </c>
       <c r="B10" t="s">
         <v>534</v>
@@ -17220,7 +17175,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>864</v>
+        <v>850</v>
       </c>
       <c r="B11" t="s">
         <v>534</v>
@@ -17231,7 +17186,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>862</v>
+        <v>848</v>
       </c>
       <c r="B12" t="s">
         <v>525</v>
@@ -17245,7 +17200,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>863</v>
+        <v>849</v>
       </c>
       <c r="B13" t="s">
         <v>528</v>
@@ -17259,7 +17214,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>863</v>
+        <v>849</v>
       </c>
       <c r="B14" t="s">
         <v>528</v>
@@ -17276,7 +17231,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>860</v>
+        <v>846</v>
       </c>
       <c r="B15" t="s">
         <v>510</v>
@@ -17287,7 +17242,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>860</v>
+        <v>846</v>
       </c>
       <c r="B16" t="s">
         <v>510</v>
@@ -17298,7 +17253,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>860</v>
+        <v>846</v>
       </c>
       <c r="B17" t="s">
         <v>510</v>
@@ -17309,7 +17264,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>865</v>
+        <v>851</v>
       </c>
       <c r="B18" t="s">
         <v>537</v>
@@ -17323,7 +17278,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>865</v>
+        <v>851</v>
       </c>
       <c r="B19" t="s">
         <v>537</v>
@@ -17343,7 +17298,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>866</v>
+        <v>852</v>
       </c>
       <c r="B20" t="s">
         <v>544</v>
@@ -17357,7 +17312,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>866</v>
+        <v>852</v>
       </c>
       <c r="B21" t="s">
         <v>544</v>
@@ -17374,7 +17329,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>866</v>
+        <v>852</v>
       </c>
       <c r="B22" t="s">
         <v>544</v>
@@ -17391,7 +17346,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>867</v>
+        <v>853</v>
       </c>
       <c r="B23" t="s">
         <v>549</v>
@@ -17405,7 +17360,7 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>867</v>
+        <v>853</v>
       </c>
       <c r="B24" t="s">
         <v>549</v>
@@ -17436,10 +17391,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17744,7 +17699,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="60">
+    <row r="38" spans="1:2" ht="48">
       <c r="A38" s="5" t="s">
         <v>639</v>
       </c>
@@ -17752,7 +17707,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="36">
+    <row r="39" spans="1:2">
       <c r="A39" s="5" t="s">
         <v>641</v>
       </c>
@@ -17760,81 +17715,25 @@
         <v>642</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="72">
+    <row r="40" spans="1:2">
       <c r="A40" s="5" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="24">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="36">
       <c r="A41" s="5" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="24">
-      <c r="A42" s="5" t="s">
-        <v>643</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="5" t="s">
-        <v>645</v>
-      </c>
-      <c r="B43" s="6" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="96">
-      <c r="A44" s="5" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
         <v>647</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="48">
-      <c r="A45" s="5" t="s">
-        <v>653</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="5" t="s">
-        <v>657</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="36">
-      <c r="A48" s="5" t="s">
-        <v>659</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>661</v>
       </c>
     </row>
   </sheetData>
@@ -17849,13 +17748,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G187"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="C84" sqref="C80:C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="4" width="28.7109375" customWidth="1"/>
     <col min="5" max="5" width="104.7109375" customWidth="1"/>
@@ -17863,7 +17762,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="60.75" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>714</v>
+        <v>700</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -17872,131 +17771,131 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>662</v>
+        <v>648</v>
       </c>
       <c r="B2" t="s">
-        <v>710</v>
+        <v>696</v>
       </c>
       <c r="C2" t="s">
-        <v>711</v>
+        <v>697</v>
       </c>
       <c r="D2" t="s">
-        <v>821</v>
+        <v>807</v>
       </c>
       <c r="E2" t="s">
-        <v>663</v>
+        <v>649</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="7" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>773</v>
+        <v>759</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="7" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>775</v>
+        <v>761</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="7" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>772</v>
+        <v>758</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="7" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>777</v>
+        <v>763</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="7" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>677</v>
+        <v>663</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>778</v>
+        <v>764</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="7" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>774</v>
+        <v>760</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="7" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>776</v>
+        <v>762</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="7" t="s">
-        <v>688</v>
+        <v>674</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -18004,10 +17903,10 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="7" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -18015,10 +17914,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="7" t="s">
-        <v>740</v>
+        <v>726</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -18026,65 +17925,65 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="7" t="s">
-        <v>707</v>
+        <v>693</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="7" t="s">
-        <v>707</v>
+        <v>693</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="7" t="s">
-        <v>707</v>
+        <v>693</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>770</v>
+        <v>756</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
       <c r="G16" t="s">
-        <v>713</v>
+        <v>699</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
-        <v>707</v>
+        <v>693</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>678</v>
+        <v>664</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
-        <v>690</v>
+        <v>676</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -18092,10 +17991,10 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
-        <v>721</v>
+        <v>707</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -18103,10 +18002,10 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
-        <v>717</v>
+        <v>703</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -18114,10 +18013,10 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
-        <v>725</v>
+        <v>711</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -18125,10 +18024,10 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
-        <v>720</v>
+        <v>706</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -18136,10 +18035,10 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
-        <v>718</v>
+        <v>704</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -18147,10 +18046,10 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="7" t="s">
-        <v>723</v>
+        <v>709</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -18158,10 +18057,10 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="7" t="s">
-        <v>726</v>
+        <v>712</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -18169,10 +18068,10 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="7" t="s">
-        <v>687</v>
+        <v>673</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -18180,10 +18079,10 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="7" t="s">
-        <v>739</v>
+        <v>725</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -18191,10 +18090,10 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="7" t="s">
-        <v>693</v>
+        <v>679</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -18202,10 +18101,10 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
-        <v>685</v>
+        <v>671</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -18213,23 +18112,23 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="7" t="s">
-        <v>666</v>
+        <v>652</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>824</v>
+        <v>810</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
-        <v>742</v>
+        <v>728</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -18237,10 +18136,10 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="7" t="s">
-        <v>697</v>
+        <v>683</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -18248,23 +18147,23 @@
     </row>
     <row r="33" spans="1:5" ht="48.75">
       <c r="A33" s="7" t="s">
-        <v>836</v>
+        <v>822</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>747</v>
+        <v>733</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8" t="s">
-        <v>837</v>
+        <v>823</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="7" t="s">
-        <v>706</v>
+        <v>692</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -18272,10 +18171,10 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="7" t="s">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -18283,10 +18182,10 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="7" t="s">
-        <v>681</v>
+        <v>667</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -18294,23 +18193,23 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="7" t="s">
-        <v>667</v>
+        <v>653</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>825</v>
+        <v>811</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="7" t="s">
-        <v>684</v>
+        <v>670</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -18318,10 +18217,10 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="7" t="s">
-        <v>686</v>
+        <v>672</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -18329,10 +18228,10 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="7" t="s">
-        <v>746</v>
+        <v>732</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>747</v>
+        <v>733</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -18340,10 +18239,10 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="7" t="s">
-        <v>743</v>
+        <v>729</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -18351,10 +18250,10 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="7" t="s">
-        <v>744</v>
+        <v>730</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
@@ -18362,10 +18261,10 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="7" t="s">
-        <v>705</v>
+        <v>691</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
@@ -18373,23 +18272,23 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="7" t="s">
-        <v>665</v>
+        <v>651</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8" t="s">
-        <v>823</v>
+        <v>809</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="7" t="s">
-        <v>734</v>
+        <v>720</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
@@ -18397,36 +18296,36 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="7" t="s">
-        <v>670</v>
+        <v>656</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>828</v>
+        <v>814</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="7" t="s">
-        <v>671</v>
+        <v>657</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>829</v>
+        <v>815</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="7" t="s">
-        <v>700</v>
+        <v>686</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -18434,10 +18333,10 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="7" t="s">
-        <v>704</v>
+        <v>690</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
@@ -18445,10 +18344,10 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="7" t="s">
-        <v>699</v>
+        <v>685</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
@@ -18456,36 +18355,36 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="7" t="s">
-        <v>672</v>
+        <v>658</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>830</v>
+        <v>816</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="7" t="s">
-        <v>675</v>
+        <v>661</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>832</v>
+        <v>818</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="7" t="s">
-        <v>702</v>
+        <v>688</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
@@ -18493,10 +18392,10 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="7" t="s">
-        <v>698</v>
+        <v>684</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
@@ -18504,36 +18403,36 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="7" t="s">
-        <v>673</v>
+        <v>659</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="8" t="s">
-        <v>834</v>
+        <v>820</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="7" t="s">
-        <v>674</v>
+        <v>660</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="8" t="s">
-        <v>831</v>
+        <v>817</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="7" t="s">
-        <v>701</v>
+        <v>687</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
@@ -18541,101 +18440,101 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="7" t="s">
-        <v>669</v>
+        <v>655</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>827</v>
+        <v>813</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="7" t="s">
-        <v>676</v>
+        <v>662</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="8" t="s">
-        <v>833</v>
+        <v>819</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="7" t="s">
-        <v>708</v>
+        <v>694</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>783</v>
+        <v>769</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="8"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="7" t="s">
-        <v>708</v>
+        <v>694</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>770</v>
+        <v>756</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="8"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="7" t="s">
-        <v>708</v>
+        <v>694</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>777</v>
+        <v>763</v>
       </c>
       <c r="D62" s="7"/>
       <c r="E62" s="8"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="7" t="s">
-        <v>708</v>
+        <v>694</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>781</v>
+        <v>767</v>
       </c>
       <c r="D63" s="7"/>
       <c r="E63" s="8"/>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="7" t="s">
-        <v>708</v>
+        <v>694</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
       <c r="D64" s="7"/>
       <c r="E64" s="8"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="7" t="s">
-        <v>683</v>
+        <v>669</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
@@ -18643,10 +18542,10 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="7" t="s">
-        <v>745</v>
+        <v>731</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>841</v>
+        <v>827</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -18654,550 +18553,550 @@
     </row>
     <row r="67" spans="1:5" ht="36.75">
       <c r="A67" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="8" t="s">
-        <v>854</v>
+        <v>840</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>797</v>
+        <v>783</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E68" s="8"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>812</v>
+        <v>798</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E69" s="8"/>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>803</v>
+        <v>789</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>847</v>
+        <v>833</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="24.75">
       <c r="A71" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>806</v>
+        <v>792</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>859</v>
+        <v>845</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>805</v>
+        <v>791</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E72" s="8"/>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>808</v>
+        <v>794</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>848</v>
+        <v>834</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>796</v>
+        <v>782</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>842</v>
+        <v>828</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>801</v>
+        <v>787</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>843</v>
+        <v>829</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>804</v>
+        <v>790</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>844</v>
+        <v>830</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>755</v>
+        <v>741</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>839</v>
+        <v>825</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>811</v>
+        <v>797</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>845</v>
+        <v>831</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>756</v>
+        <v>742</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>846</v>
+        <v>832</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>849</v>
+        <v>835</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>760</v>
+        <v>746</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>850</v>
+        <v>836</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>758</v>
+        <v>744</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>851</v>
+        <v>837</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>759</v>
+        <v>745</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>852</v>
+        <v>838</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>761</v>
+        <v>747</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>853</v>
+        <v>839</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>802</v>
+        <v>788</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>855</v>
+        <v>841</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>665</v>
+        <v>651</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>856</v>
+        <v>842</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>799</v>
+        <v>785</v>
       </c>
       <c r="D87" s="7"/>
       <c r="E87" s="8" t="s">
-        <v>857</v>
+        <v>843</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>858</v>
+        <v>844</v>
       </c>
       <c r="D88" s="7"/>
       <c r="E88" s="8"/>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>820</v>
+        <v>806</v>
       </c>
       <c r="D89" s="7"/>
       <c r="E89" s="8"/>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>810</v>
+        <v>796</v>
       </c>
       <c r="D90" s="7"/>
       <c r="E90" s="8"/>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>818</v>
+        <v>804</v>
       </c>
       <c r="D91" s="7"/>
       <c r="E91" s="8"/>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>816</v>
+        <v>802</v>
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="8"/>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>815</v>
+        <v>801</v>
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="8"/>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>817</v>
+        <v>803</v>
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="8"/>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>809</v>
+        <v>795</v>
       </c>
       <c r="D95" s="7"/>
       <c r="E95" s="8"/>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>819</v>
+        <v>805</v>
       </c>
       <c r="D96" s="7"/>
       <c r="E96" s="8"/>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>814</v>
+        <v>800</v>
       </c>
       <c r="D97" s="7"/>
       <c r="E97" s="8"/>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>813</v>
+        <v>799</v>
       </c>
       <c r="D98" s="7"/>
       <c r="E98" s="8"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>807</v>
+        <v>793</v>
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="8"/>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>798</v>
+        <v>784</v>
       </c>
       <c r="D100" s="7"/>
       <c r="E100" s="8"/>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>677</v>
+        <v>663</v>
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="8"/>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="7" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>800</v>
+        <v>786</v>
       </c>
       <c r="D102" s="7"/>
       <c r="E102" s="8"/>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="7" t="s">
-        <v>722</v>
+        <v>708</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
@@ -19205,10 +19104,10 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="7" t="s">
-        <v>719</v>
+        <v>705</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
@@ -19216,10 +19115,10 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="7" t="s">
-        <v>724</v>
+        <v>710</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
@@ -19227,10 +19126,10 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="7" t="s">
-        <v>727</v>
+        <v>713</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
@@ -19238,10 +19137,10 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="7" t="s">
-        <v>682</v>
+        <v>668</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
@@ -19249,10 +19148,10 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="7" t="s">
-        <v>695</v>
+        <v>681</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
@@ -19260,10 +19159,10 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="7" t="s">
-        <v>741</v>
+        <v>727</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
@@ -19271,23 +19170,23 @@
     </row>
     <row r="110" spans="1:5" ht="36.75">
       <c r="A110" s="7" t="s">
-        <v>664</v>
+        <v>650</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="8" t="s">
-        <v>822</v>
+        <v>808</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="7" t="s">
-        <v>703</v>
+        <v>689</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
@@ -19295,114 +19194,114 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="7" t="s">
-        <v>709</v>
+        <v>695</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>687</v>
+        <v>673</v>
       </c>
       <c r="D112" s="7"/>
       <c r="E112" s="8"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="7" t="s">
-        <v>709</v>
+        <v>695</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>770</v>
+        <v>756</v>
       </c>
       <c r="D113" s="7"/>
       <c r="E113" s="8"/>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="7" t="s">
-        <v>709</v>
+        <v>695</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>785</v>
+        <v>771</v>
       </c>
       <c r="D114" s="7"/>
       <c r="E114" s="8"/>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="7" t="s">
-        <v>709</v>
+        <v>695</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>786</v>
+        <v>772</v>
       </c>
       <c r="D115" s="7"/>
       <c r="E115" s="8"/>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="7" t="s">
-        <v>709</v>
+        <v>695</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>769</v>
+        <v>755</v>
       </c>
       <c r="D116" s="7"/>
       <c r="E116" s="8"/>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="7" t="s">
-        <v>709</v>
+        <v>695</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>784</v>
+        <v>770</v>
       </c>
       <c r="D117" s="7"/>
       <c r="E117" s="8"/>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="7" t="s">
-        <v>709</v>
+        <v>695</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>691</v>
+        <v>677</v>
       </c>
       <c r="D118" s="7"/>
       <c r="E118" s="8"/>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="7" t="s">
-        <v>709</v>
+        <v>695</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>787</v>
+        <v>773</v>
       </c>
       <c r="D119" s="7"/>
       <c r="E119" s="8"/>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="7" t="s">
-        <v>731</v>
+        <v>717</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
@@ -19410,10 +19309,10 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="7" t="s">
-        <v>730</v>
+        <v>716</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
@@ -19421,10 +19320,10 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="7" t="s">
-        <v>732</v>
+        <v>718</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
@@ -19432,10 +19331,10 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="7" t="s">
-        <v>733</v>
+        <v>719</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
@@ -19443,10 +19342,10 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="7" t="s">
-        <v>728</v>
+        <v>714</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
@@ -19454,10 +19353,10 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="7" t="s">
-        <v>729</v>
+        <v>715</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
@@ -19465,23 +19364,23 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="7" t="s">
-        <v>677</v>
+        <v>663</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
       <c r="E126" s="8" t="s">
-        <v>835</v>
+        <v>821</v>
       </c>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="7" t="s">
-        <v>738</v>
+        <v>724</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
@@ -19489,10 +19388,10 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="7" t="s">
-        <v>736</v>
+        <v>722</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
@@ -19500,10 +19399,10 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="7" t="s">
-        <v>737</v>
+        <v>723</v>
       </c>
       <c r="B129" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C129" s="7"/>
       <c r="D129" s="7"/>
@@ -19511,413 +19410,413 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C130" s="7" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
       <c r="D130" s="7"/>
       <c r="E130" s="8"/>
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>789</v>
+        <v>775</v>
       </c>
       <c r="D131" s="7"/>
       <c r="E131" s="8"/>
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>740</v>
+        <v>726</v>
       </c>
       <c r="D132" s="7"/>
       <c r="E132" s="8"/>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>739</v>
+        <v>725</v>
       </c>
       <c r="D133" s="7"/>
       <c r="E133" s="8"/>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>742</v>
+        <v>728</v>
       </c>
       <c r="D134" s="7"/>
       <c r="E134" s="8"/>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>686</v>
+        <v>672</v>
       </c>
       <c r="D135" s="7"/>
       <c r="E135" s="8"/>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>792</v>
+        <v>778</v>
       </c>
       <c r="D136" s="7"/>
       <c r="E136" s="8"/>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>743</v>
+        <v>729</v>
       </c>
       <c r="D137" s="7"/>
       <c r="E137" s="8"/>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>791</v>
+        <v>777</v>
       </c>
       <c r="D138" s="7"/>
       <c r="E138" s="8"/>
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>795</v>
+        <v>781</v>
       </c>
       <c r="D139" s="7"/>
       <c r="E139" s="8"/>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>744</v>
+        <v>730</v>
       </c>
       <c r="D140" s="7"/>
       <c r="E140" s="8"/>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C141" s="7" t="s">
-        <v>794</v>
+        <v>780</v>
       </c>
       <c r="D141" s="7"/>
       <c r="E141" s="8"/>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>793</v>
+        <v>779</v>
       </c>
       <c r="D142" s="7"/>
       <c r="E142" s="8"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>790</v>
+        <v>776</v>
       </c>
       <c r="D143" s="7"/>
       <c r="E143" s="8"/>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B144" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>700</v>
+        <v>686</v>
       </c>
       <c r="D144" s="7"/>
       <c r="E144" s="8"/>
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B145" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>704</v>
+        <v>690</v>
       </c>
       <c r="D145" s="7"/>
       <c r="E145" s="8"/>
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>699</v>
+        <v>685</v>
       </c>
       <c r="D146" s="7"/>
       <c r="E146" s="8"/>
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C147" s="7" t="s">
-        <v>702</v>
+        <v>688</v>
       </c>
       <c r="D147" s="7"/>
       <c r="E147" s="8"/>
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B148" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C148" s="7" t="s">
-        <v>698</v>
+        <v>684</v>
       </c>
       <c r="D148" s="7"/>
       <c r="E148" s="8"/>
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C149" s="7" t="s">
-        <v>701</v>
+        <v>687</v>
       </c>
       <c r="D149" s="7"/>
       <c r="E149" s="8"/>
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>741</v>
+        <v>727</v>
       </c>
       <c r="D150" s="7"/>
       <c r="E150" s="8"/>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C151" s="7" t="s">
-        <v>703</v>
+        <v>689</v>
       </c>
       <c r="D151" s="7"/>
       <c r="E151" s="8"/>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="7" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
       <c r="C152" s="7" t="s">
-        <v>678</v>
+        <v>664</v>
       </c>
       <c r="D152" s="7"/>
       <c r="E152" s="8"/>
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="7" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C153" s="7" t="s">
-        <v>767</v>
+        <v>753</v>
       </c>
       <c r="D153" s="7"/>
       <c r="E153" s="8"/>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="7" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C154" s="7" t="s">
-        <v>768</v>
+        <v>754</v>
       </c>
       <c r="D154" s="7"/>
       <c r="E154" s="8"/>
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="7" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C155" s="7" t="s">
-        <v>687</v>
+        <v>673</v>
       </c>
       <c r="D155" s="7"/>
       <c r="E155" s="8"/>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="7" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C156" s="7" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="D156" s="7"/>
       <c r="E156" s="8"/>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="7" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C157" s="7" t="s">
-        <v>770</v>
+        <v>756</v>
       </c>
       <c r="D157" s="7"/>
       <c r="E157" s="8"/>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="7" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C158" s="7" t="s">
-        <v>769</v>
+        <v>755</v>
       </c>
       <c r="D158" s="7"/>
       <c r="E158" s="8"/>
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="7" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C159" s="7" t="s">
-        <v>771</v>
+        <v>757</v>
       </c>
       <c r="D159" s="7"/>
       <c r="E159" s="8"/>
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="7" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C160" s="7" t="s">
-        <v>691</v>
+        <v>677</v>
       </c>
       <c r="D160" s="7"/>
       <c r="E160" s="8"/>
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="7" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C161" s="7"/>
       <c r="D161" s="7"/>
@@ -19925,10 +19824,10 @@
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="7" t="s">
-        <v>691</v>
+        <v>677</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C162" s="7"/>
       <c r="D162" s="7"/>
@@ -19936,10 +19835,10 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="7" t="s">
-        <v>735</v>
+        <v>721</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C163" s="7"/>
       <c r="D163" s="7"/>
@@ -19947,183 +19846,183 @@
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="7" t="s">
-        <v>668</v>
+        <v>654</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
       <c r="E164" s="8" t="s">
-        <v>826</v>
+        <v>812</v>
       </c>
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="7" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C165" s="7" t="s">
-        <v>755</v>
+        <v>741</v>
       </c>
       <c r="D165" s="7"/>
       <c r="E165" s="8" t="s">
-        <v>839</v>
+        <v>825</v>
       </c>
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="7" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C166" s="7" t="s">
-        <v>756</v>
+        <v>742</v>
       </c>
       <c r="D166" s="7"/>
       <c r="E166" s="8" t="s">
-        <v>840</v>
+        <v>826</v>
       </c>
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="7" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C167" s="7" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="D167" s="7"/>
       <c r="E167" s="8"/>
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="7" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C168" s="7" t="s">
-        <v>760</v>
+        <v>746</v>
       </c>
       <c r="D168" s="7"/>
       <c r="E168" s="8"/>
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="7" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C169" s="7" t="s">
-        <v>758</v>
+        <v>744</v>
       </c>
       <c r="D169" s="7"/>
       <c r="E169" s="8"/>
     </row>
     <row r="170" spans="1:5">
       <c r="A170" s="7" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C170" s="7" t="s">
-        <v>759</v>
+        <v>745</v>
       </c>
       <c r="D170" s="7"/>
       <c r="E170" s="8"/>
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="7" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C171" s="7" t="s">
-        <v>761</v>
+        <v>747</v>
       </c>
       <c r="D171" s="7"/>
       <c r="E171" s="8"/>
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="7" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C172" s="7" t="s">
-        <v>665</v>
+        <v>651</v>
       </c>
       <c r="D172" s="7"/>
       <c r="E172" s="8"/>
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="7" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C173" s="7" t="s">
-        <v>677</v>
+        <v>663</v>
       </c>
       <c r="D173" s="7"/>
       <c r="E173" s="8"/>
     </row>
     <row r="174" spans="1:5">
       <c r="A174" s="7" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C174" s="7" t="s">
-        <v>764</v>
+        <v>750</v>
       </c>
       <c r="D174" s="7"/>
       <c r="E174" s="8"/>
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="7" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C175" s="7" t="s">
-        <v>762</v>
+        <v>748</v>
       </c>
       <c r="D175" s="7"/>
       <c r="E175" s="8"/>
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="7" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="B176" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C176" s="7" t="s">
-        <v>763</v>
+        <v>749</v>
       </c>
       <c r="D176" s="7"/>
       <c r="E176" s="8"/>
     </row>
     <row r="177" spans="1:5">
       <c r="A177" s="7" t="s">
-        <v>679</v>
+        <v>665</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C177" s="9">
         <v>2012</v>
@@ -20133,10 +20032,10 @@
     </row>
     <row r="178" spans="1:5">
       <c r="A178" s="7" t="s">
-        <v>679</v>
+        <v>665</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C178" s="10">
         <v>2013</v>
@@ -20146,88 +20045,88 @@
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="7" t="s">
-        <v>679</v>
+        <v>665</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>751</v>
+        <v>737</v>
       </c>
       <c r="D179" s="7"/>
       <c r="E179" s="8"/>
     </row>
     <row r="180" spans="1:5">
       <c r="A180" s="7" t="s">
-        <v>679</v>
+        <v>665</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>753</v>
+        <v>739</v>
       </c>
       <c r="D180" s="7"/>
       <c r="E180" s="8"/>
     </row>
     <row r="181" spans="1:5">
       <c r="A181" s="7" t="s">
-        <v>679</v>
+        <v>665</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>665</v>
+        <v>651</v>
       </c>
       <c r="D181" s="7"/>
       <c r="E181" s="8"/>
     </row>
     <row r="182" spans="1:5">
       <c r="A182" s="7" t="s">
-        <v>679</v>
+        <v>665</v>
       </c>
       <c r="B182" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C182" s="9" t="s">
-        <v>750</v>
+        <v>736</v>
       </c>
       <c r="D182" s="7"/>
       <c r="E182" s="8"/>
     </row>
     <row r="183" spans="1:5">
       <c r="A183" s="7" t="s">
-        <v>679</v>
+        <v>665</v>
       </c>
       <c r="B183" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C183" s="9" t="s">
-        <v>752</v>
+        <v>738</v>
       </c>
       <c r="D183" s="7"/>
       <c r="E183" s="8"/>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="7" t="s">
-        <v>679</v>
+        <v>665</v>
       </c>
       <c r="B184" s="7" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="C184" s="9" t="s">
-        <v>754</v>
+        <v>740</v>
       </c>
       <c r="D184" s="7"/>
       <c r="E184" s="8"/>
     </row>
     <row r="185" spans="1:5">
       <c r="A185" s="7" t="s">
-        <v>694</v>
+        <v>680</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C185" s="7"/>
       <c r="D185" s="7"/>
@@ -20235,23 +20134,23 @@
     </row>
     <row r="186" spans="1:5">
       <c r="A186" s="7" t="s">
-        <v>678</v>
+        <v>664</v>
       </c>
       <c r="B186" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C186" s="7"/>
       <c r="D186" s="7"/>
       <c r="E186" s="8" t="s">
-        <v>838</v>
+        <v>824</v>
       </c>
     </row>
     <row r="187" spans="1:5">
       <c r="A187" s="7" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="C187" s="7"/>
       <c r="D187" s="7"/>

</xml_diff>